<commit_message>
Plotly and Machine Learning
</commit_message>
<xml_diff>
--- a/nba_finals_locations.xlsx
+++ b/nba_finals_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\HW\Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBE8F23-79D2-4894-AF64-2C77F56F5335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27DDE04-B090-47CC-878C-1683939B7AA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6B02A2C6-7C87-4916-B039-17A0587A249A}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>

</xml_diff>